<commit_message>
aggiornato report-checklist.xlsx id: 31,39,47,75,76,77,78,79,80,81,82,83,84,85,86,87,88,89,90,91,92,93 con colonna TEST AUTOCERTIFICATO a SI
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111ELCO0000000/EL_CO_/Fenix/v3_19_05/report-checklist.xlsx
+++ b/GATEWAY/A1#111ELCO0000000/EL_CO_/Fenix/v3_19_05/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio.capra\Desktop\ACCREDITAMENTO\ACCREDITAMENTO_FSE\it-fse-accreditamento\GATEWAY\A1#111ELCO0000000\EL_CO_\Fenix\v3_19_05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F28BC6F-B5FB-4D14-809D-88F753CD30A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D335DB30-7080-4B21-9EE5-A55E11320727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5385" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prerequisiti" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="420">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -4022,10 +4022,10 @@
   <dimension ref="A1:O992"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E89" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E90" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="L90" sqref="L90:L92"/>
+      <selection pane="bottomRight" activeCell="N94" sqref="N94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5043,7 +5043,9 @@
         <v>318</v>
       </c>
       <c r="M37" s="19"/>
-      <c r="N37" s="20"/>
+      <c r="N37" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="O37" s="21"/>
     </row>
     <row r="38" spans="1:15" ht="120" hidden="1">
@@ -5229,7 +5231,9 @@
         <v>318</v>
       </c>
       <c r="M43" s="19"/>
-      <c r="N43" s="20"/>
+      <c r="N43" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="O43" s="21"/>
     </row>
     <row r="44" spans="1:15" ht="135" hidden="1">
@@ -5409,7 +5413,9 @@
         <v>318</v>
       </c>
       <c r="M49" s="19"/>
-      <c r="N49" s="20"/>
+      <c r="N49" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="O49" s="21"/>
     </row>
     <row r="50" spans="1:15" ht="45" hidden="1">
@@ -6204,7 +6210,9 @@
         <v>318</v>
       </c>
       <c r="M76" s="19"/>
-      <c r="N76" s="20"/>
+      <c r="N76" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="O76" s="39" t="s">
         <v>342</v>
       </c>
@@ -6247,7 +6255,9 @@
         <v>318</v>
       </c>
       <c r="M77" s="19"/>
-      <c r="N77" s="20"/>
+      <c r="N77" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="O77" s="39" t="s">
         <v>347</v>
       </c>
@@ -6290,7 +6300,9 @@
         <v>318</v>
       </c>
       <c r="M78" s="19"/>
-      <c r="N78" s="20"/>
+      <c r="N78" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="O78" s="39" t="s">
         <v>352</v>
       </c>
@@ -6333,7 +6345,9 @@
         <v>318</v>
       </c>
       <c r="M79" s="19"/>
-      <c r="N79" s="20"/>
+      <c r="N79" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="O79" s="39" t="s">
         <v>357</v>
       </c>
@@ -6376,7 +6390,9 @@
         <v>318</v>
       </c>
       <c r="M80" s="19"/>
-      <c r="N80" s="20"/>
+      <c r="N80" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="O80" s="39" t="s">
         <v>359</v>
       </c>
@@ -6419,7 +6435,9 @@
         <v>318</v>
       </c>
       <c r="M81" s="19"/>
-      <c r="N81" s="20"/>
+      <c r="N81" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="O81" s="39" t="s">
         <v>361</v>
       </c>
@@ -6462,7 +6480,9 @@
         <v>318</v>
       </c>
       <c r="M82" s="19"/>
-      <c r="N82" s="20"/>
+      <c r="N82" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="O82" s="39" t="s">
         <v>365</v>
       </c>
@@ -6505,7 +6525,9 @@
         <v>318</v>
       </c>
       <c r="M83" s="19"/>
-      <c r="N83" s="20"/>
+      <c r="N83" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="O83" s="39" t="s">
         <v>383</v>
       </c>
@@ -6548,7 +6570,9 @@
         <v>318</v>
       </c>
       <c r="M84" s="19"/>
-      <c r="N84" s="20"/>
+      <c r="N84" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="O84" s="21" t="s">
         <v>388</v>
       </c>
@@ -6591,7 +6615,9 @@
         <v>318</v>
       </c>
       <c r="M85" s="19"/>
-      <c r="N85" s="20"/>
+      <c r="N85" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="O85" s="21" t="s">
         <v>393</v>
       </c>
@@ -6634,7 +6660,9 @@
         <v>318</v>
       </c>
       <c r="M86" s="19"/>
-      <c r="N86" s="20"/>
+      <c r="N86" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="O86" s="21" t="s">
         <v>398</v>
       </c>
@@ -6677,7 +6705,9 @@
         <v>318</v>
       </c>
       <c r="M87" s="19"/>
-      <c r="N87" s="20"/>
+      <c r="N87" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="O87" s="21" t="s">
         <v>403</v>
       </c>
@@ -6720,7 +6750,9 @@
         <v>318</v>
       </c>
       <c r="M88" s="19"/>
-      <c r="N88" s="20"/>
+      <c r="N88" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="O88" s="21"/>
     </row>
     <row r="89" spans="1:15" ht="120.75" thickBot="1">
@@ -6761,7 +6793,9 @@
         <v>318</v>
       </c>
       <c r="M89" s="19"/>
-      <c r="N89" s="20"/>
+      <c r="N89" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="O89" s="21"/>
     </row>
     <row r="90" spans="1:15" ht="105">
@@ -6794,7 +6828,9 @@
       <c r="M90" s="37" t="s">
         <v>412</v>
       </c>
-      <c r="N90" s="20"/>
+      <c r="N90" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="O90" s="21"/>
     </row>
     <row r="91" spans="1:15" ht="105">
@@ -6827,7 +6863,9 @@
       <c r="M91" s="37" t="s">
         <v>419</v>
       </c>
-      <c r="N91" s="20"/>
+      <c r="N91" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="O91" s="21"/>
     </row>
     <row r="92" spans="1:15" ht="120">
@@ -6860,7 +6898,9 @@
       <c r="M92" s="37" t="s">
         <v>419</v>
       </c>
-      <c r="N92" s="20"/>
+      <c r="N92" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="O92" s="21"/>
     </row>
     <row r="93" spans="1:15" ht="120.75" thickBot="1">
@@ -6901,7 +6941,9 @@
         <v>318</v>
       </c>
       <c r="M93" s="19"/>
-      <c r="N93" s="20"/>
+      <c r="N93" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="O93" s="21"/>
     </row>
     <row r="94" spans="1:15" ht="150">
@@ -6942,7 +6984,9 @@
         <v>318</v>
       </c>
       <c r="M94" s="19"/>
-      <c r="N94" s="20"/>
+      <c r="N94" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="O94" s="21"/>
     </row>
     <row r="95" spans="1:15" ht="14.25" hidden="1" customHeight="1">

</xml_diff>

<commit_message>
Rimossa Colonna F in quanto non applicabile (le altre erano già vuote) ai punti 89,90,91
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111ELCO0000000/EL_CO_/Fenix/v3_19_05/report-checklist.xlsx
+++ b/GATEWAY/A1#111ELCO0000000/EL_CO_/Fenix/v3_19_05/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio.capra\Desktop\ACCREDITAMENTO\ACCREDITAMENTO_FSE\it-fse-accreditamento\GATEWAY\A1#111ELCO0000000\EL_CO_\Fenix\v3_19_05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D335DB30-7080-4B21-9EE5-A55E11320727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBE2D83-B025-4B48-AEF5-801798870F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prerequisiti" sheetId="1" r:id="rId1"/>
@@ -4022,10 +4022,10 @@
   <dimension ref="A1:O992"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E90" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E86" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="N94" sqref="N94"/>
+      <selection pane="bottomRight" activeCell="G92" sqref="G92:I92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -6814,9 +6814,7 @@
       <c r="E90" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="F90" s="17">
-        <v>44970</v>
-      </c>
+      <c r="F90" s="17"/>
       <c r="G90" s="18"/>
       <c r="H90" s="18"/>
       <c r="I90" s="18"/>
@@ -6849,9 +6847,7 @@
       <c r="E91" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="F91" s="17">
-        <v>44970</v>
-      </c>
+      <c r="F91" s="17"/>
       <c r="G91" s="18"/>
       <c r="H91" s="18"/>
       <c r="I91" s="18"/>
@@ -6884,9 +6880,7 @@
       <c r="E92" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="F92" s="17">
-        <v>44970</v>
-      </c>
+      <c r="F92" s="17"/>
       <c r="G92" s="18"/>
       <c r="H92" s="18"/>
       <c r="I92" s="18"/>

</xml_diff>

<commit_message>
Migliorata qualità pdf e aggiunti campi del cda dentro il pdf
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111ELCO0000000/EL_CO_/Fenix/v3_19_05/report-checklist.xlsx
+++ b/GATEWAY/A1#111ELCO0000000/EL_CO_/Fenix/v3_19_05/report-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio.capra\Desktop\ACCREDITAMENTO\ACCREDITAMENTO_FSE\it-fse-accreditamento\GATEWAY\A1#111ELCO0000000\EL_CO_\Fenix\v3_19_05\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio.capra\Desktop\ACCREDITAMENTO\A1#111ELCO0000000\EL_CO_\Fenix\v3_19_05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBE2D83-B025-4B48-AEF5-801798870F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9883D6-7FD7-424F-8503-91E40FED603A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="5385" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prerequisiti" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="421">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -1742,24 +1742,6 @@
     <t>NO</t>
   </si>
   <si>
-    <t>2023-02-13T08:31:01.231Z</t>
-  </si>
-  <si>
-    <t>2dd133f8392fa40e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.1987792b2bd7eabc8ae32044ae56988ec3700ef4acdc03aa137eef723cdfb426.8acd9c15d8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-13T08:41:21.044Z</t>
-  </si>
-  <si>
-    <t>11d7adf3cb93a333</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.86bc5e507d4d5dc151e070cee6b1657e7f77a844937cd91e8e6fe43cd33962f7.f727f5fb51^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Il sistema attende un numero di millisecondi configurabile (default 5000) Dopo tale tempo viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
   </si>
   <si>
@@ -1815,12 +1797,6 @@
     <t>Inserita storia clinica testuale non gestita anamnesi familiare</t>
   </si>
   <si>
-    <t>2023-02-13T11:58:51.448Z</t>
-  </si>
-  <si>
-    <t>6a9f89b3c8788409</t>
-  </si>
-  <si>
     <t>detail:"Il campo person_id non è valorizzato"
 error:"Il campo person_id non è valorizzato"
 instance:"/jwt-mandatory-field-missing"
@@ -1838,19 +1814,6 @@
     <t>Essendo il codice fiscale del paziente inserito nel jwt per l'autenticazione viene ritornato un errore 403 in quanto il jwt non risulta valido</t>
   </si>
   <si>
-    <t>2023-02-13T13:36:43.665Z</t>
-  </si>
-  <si>
-    <t>7b26c3e441ad23bc</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.758c72330f0cc75f13b29742b0b471451ded05997469069d497095e29c93ad48.d468c57f0e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>[Errore-46| codice fiscale 'RSSMRA75C03F839k' cittadino ed operatore: 16 cifre [A-Z0-9]{16}] 
-Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo ed obbligare l'operatore a coreggere l'errore o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
-  </si>
-  <si>
     <t>Viene simulato da db in quanto l'applicativo registra sempre con upper case nel campo codice fiscale</t>
   </si>
   <si>
@@ -1858,25 +1821,7 @@
 Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo ed obbligare l'operatore a coreggere l'errore o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.758c72330f0cc75f13b29742b0b471451ded05997469069d497095e29c93ad48.9ee36286e5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>eb928d2bdb698835</t>
-  </si>
-  <si>
-    <t>2023-02-13T13:47:33.666Z</t>
-  </si>
-  <si>
     <t>Generato da db. I documenti possono essere solo classificati come N o V</t>
-  </si>
-  <si>
-    <t>2023-02-13T13:56:26.968Z</t>
-  </si>
-  <si>
-    <t>f26ed1fdafc7340b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.758c72330f0cc75f13b29742b0b471451ded05997469069d497095e29c93ad48.b0320f3e57^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>[ERRORE-11| L'elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i suoi sotto-elementi 'country', 'city' e 'streetAddressLine'.   ]
@@ -1900,12 +1845,6 @@
     <t>Generato da database levando costraint su sesso</t>
   </si>
   <si>
-    <t>1216fbff6f557cc7</t>
-  </si>
-  <si>
-    <t>2023-02-13T16:01:02.933Z</t>
-  </si>
-  <si>
     <t>[ERRORE-40| L'elemento ClinicalDocument/documentationOf/serviceEvent deve contenere l'elemento code e DEVE valorizzare il suo attributo code con uno dei seguenti valori: 'PROG'|'DIR'|'RAD_PROG|'RAD_DIR' ]
 Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo ed obbligare l'operatore a coreggere l'errore o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
   </si>
@@ -1913,54 +1852,6 @@
     <t>Generato da database levando costraint su tipo accesso</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.758c72330f0cc75f13b29742b0b471451ded05997469069d497095e29c93ad48.cf1271a813^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>594efc4050baa0c5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.758c72330f0cc75f13b29742b0b471451ded05997469069d497095e29c93ad48.52f3856c68^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-13T16:10:42.157Z</t>
-  </si>
-  <si>
-    <t>d9703abd28fb6ab2</t>
-  </si>
-  <si>
-    <t>2023-02-13T16:13:22.869Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.758c72330f0cc75f13b29742b0b471451ded05997469069d497095e29c93ad48.b957430925^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.fc274157e51e8b85203e39c14dac8641c832293d1ab05ea14f2f036fdc2414ce.cbaaf3809b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-13T16:32:00.789Z</t>
-  </si>
-  <si>
-    <t>7c537c45579caf86</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.014797e9a5876e8866bba025192c753fdfaad36c0745d6ed26e2d971e11acc85.c30963bb13^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>4cbf82d26677ded1</t>
-  </si>
-  <si>
-    <t>2023-02-13T16:38:56.700Z</t>
-  </si>
-  <si>
-    <t>2023-02-13T16:45:23.632Z</t>
-  </si>
-  <si>
-    <t>806ccc2b435106cd</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.758c72330f0cc75f13b29742b0b471451ded05997469069d497095e29c93ad48.1c529bccd0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>[ERRORE-39| inFulfillmentOf/order/priorityCode DEVE avere l'attributo '@codeSystem='2.16.840.1.113883.5.7' e @code valorizzato con uno dei seguenti valori: 'R'|'P'|'UR'|'EM' ],[ERRORE-39| inFulfillmentOf/order/priorityCode DEVE avere l'attributo '@codeSystem='2.16.840.1.113883.5.7' e @code valorizzato con uno dei seguenti valori: 'R'|'P'|'UR'|'EM' ]
 Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo ed obbligare l'operatore a coreggere l'errore o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
   </si>
@@ -1968,15 +1859,6 @@
     <t>Generato da database levando costraint su priorità</t>
   </si>
   <si>
-    <t>2023-02-13T16:51:15.413Z</t>
-  </si>
-  <si>
-    <t>388a101c0f4d801f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.758c72330f0cc75f13b29742b0b471451ded05997469069d497095e29c93ad48.069440e493^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element 'priorityCode'. One of '{"urn:hl7-org:v3":realmCode, "urn:hl7-org:v3":typeId, "urn:hl7-org:v3":templateId, "urn:hl7-org:v3":id}' is expected.,ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element 'priorityCode'. One of '{"urn:hl7-org:v3":realmCode, "urn:hl7-org:v3":typeId, "urn:hl7-org:v3":templateId, "urn:hl7-org:v3":id}' is expected.
 Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo ed obbligare l'operatore a coreggere l'errore o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
   </si>
@@ -1984,15 +1866,6 @@
     <t>Generato da db l'id è obbligatorio</t>
   </si>
   <si>
-    <t>2023-02-13T16:55:43.733Z</t>
-  </si>
-  <si>
-    <t>e5ed7cb62afc5613</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.758c72330f0cc75f13b29742b0b471451ded05997469069d497095e29c93ad48.1d2a77a05a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element 'text'. One of '{"urn:hl7-org:v3":realmCode, "urn:hl7-org:v3":typeId, "urn:hl7-org:v3":templateId, "urn:hl7-org:v3":id, "urn:hl7-org:v3":code}' is expected.
 Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo ed obbligare l'operatore a coreggere l'errore o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
   </si>
@@ -2000,15 +1873,6 @@
     <t>Forzato da database. Almeno un esame deve essere eseguito per generare un referto</t>
   </si>
   <si>
-    <t xml:space="preserve"> 2023-02-13T17:00:22.467Z</t>
-  </si>
-  <si>
-    <t>d0ede60e53d09c58</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.758c72330f0cc75f13b29742b0b471451ded05997469069d497095e29c93ad48.7428ec7b7a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>[ERRORE-b5| Sezione Referto: La sezione deve contenere l'elemento 'text'.]
 Impossibile continuare senza referto</t>
   </si>
@@ -2016,15 +1880,6 @@
     <t>Impossibile generare il referto senza testo</t>
   </si>
   <si>
-    <t>2023-02-13T17:04:08.082Z</t>
-  </si>
-  <si>
-    <t>b69ac149fe688555</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.758c72330f0cc75f13b29742b0b471451ded05997469069d497095e29c93ad48.3fd173a733^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>[ERRORE-b13| Sezione Precedenti Esami Eseguiti: La section deve contenere l'elemento 'text'.]
 Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo ed obbligare l'operatore a coreggere l'errore o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
   </si>
@@ -2032,24 +1887,6 @@
     <t>Se non presenti precedenti viene rimosso l'intero componet. Forzato errore</t>
   </si>
   <si>
-    <t>5f034d90e6765f5d</t>
-  </si>
-  <si>
-    <t>2023-02-13T17:10:16.818Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.89759a3fa41e8673b7e4e6f563198d5ec08766043e2e424357352a73d996df08.3494902eb0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-13T17:15:36.182Z</t>
-  </si>
-  <si>
-    <t>77c0d701fbd9b3ab</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.e83ce8cbb4f8a63707c80470076808609c75c3acf44a3c91cdc4e5a362779901.8d39f85b4c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>[ERRORE-b7| Sezione Dicom Object Catalog: La sezione deve avere l'elemento 'entry' di tipo 'act'.]
 Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo ed obbligare l'operatore a coreggere l'errore o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
   </si>
@@ -2061,26 +1898,211 @@
     <t>Non viene gestita l'anamnesi familiare strutturata  sul ris</t>
   </si>
   <si>
-    <t>2d08b1c13e74bf0f</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2023-02-13T17:32:57.198Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.e83ce8cbb4f8a63707c80470076808609c75c3acf44a3c91cdc4e5a362779901.3616a668ff^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.6.103, Codes: XYZ]
 Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo ed obbligare l'operatore a coreggere l'errore o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
   </si>
   <si>
-    <t>40cdedd59700ff01</t>
-  </si>
-  <si>
-    <t>2023-02-13T17:32:57.198Z</t>
-  </si>
-  <si>
     <t>Non vengono gestite le allergie codificate secondo catologo</t>
+  </si>
+  <si>
+    <t>2023-03-05T09:49:20.669Z</t>
+  </si>
+  <si>
+    <t>0d853d260d8da95a</t>
+  </si>
+  <si>
+    <r>
+      <t>[Errore-46| codice fiscale '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CCRSTS82A01B369q</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>' cittadino ed operatore: 16 cifre [A-Z0-9]{16}] 
+Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo ed obbligare l'operatore a coreggere l'errore o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
+    </r>
+  </si>
+  <si>
+    <t>2023-03-05T15:15:33.784Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.fac9100ff805213589f0ce61b9e113ade69245c7d4a32580aa45a781adf14a85.659f03b2bd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>8857858bafc0cdcb</t>
+  </si>
+  <si>
+    <t>2023-03-05T15:19:21.453Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.e1d40865d22f3646c2624681e600530948f1f5eef570a671f4d6c4e788744609.695dfff480^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>1696474b49700d23</t>
+  </si>
+  <si>
+    <t>2023-03-05T15:43:59.488Z</t>
+  </si>
+  <si>
+    <t>58984d7d30148227</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.61c4e0872a7c760646136b5caa696a1f5ec0b74b8c7f4a284cca969e1562bb44.821d0a7b83^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-05T15:48:26.345Z</t>
+  </si>
+  <si>
+    <t>5e755f4676c6447c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.67841ce84ac54216063e2af32be49d48b13fa8762ad64d2d78b8597357463ba2.fa3de537db^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-05T15:52:23.963Z</t>
+  </si>
+  <si>
+    <t>6cad2893193932c4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.c625c7edbdc8d03c4d6889de92330e92bba14233d3c521e4ae929a3f15652d89.2b0a582a36^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-05T15:55:36.429Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.93c8a931216913206390699d605be93400670a9983ef65b462b088814ac2295e.5fba1727f0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>25232b73b087bf1e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.3d0b1b6b6700c28b7fc6c16797593d3da15bb35393abe1e11445de8fc3afd2b2.dd83fa9d6c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-05T16:18:56.048Z</t>
+  </si>
+  <si>
+    <t>1601ab9378170c8c</t>
+  </si>
+  <si>
+    <t>2023-03-05T16:22:44.712Z</t>
+  </si>
+  <si>
+    <t>dcc32c7d926c42e9</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.f80c465682d09695c9234ea6ddc892e2f01db64acf4d1dbdd5385c50ec6a0962.e082c84b9a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-05T16:29:05.815Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.cdb593d9483f1f0aa1ff398d8216d67146f506dfccecb880fcf51bce038fdb7f.f608f0558c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>ca555288012b3c10</t>
+  </si>
+  <si>
+    <t>2023-03-05T16:33:00.390Z</t>
+  </si>
+  <si>
+    <t>28df54934e6acf96</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.505feba206f26f2e23008e608176d780a1cf09ecab0a4fc75c534e605e76b458.9bca3ff902^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-05T16:40:58.474Z</t>
+  </si>
+  <si>
+    <t>f0b1bbff29de15b4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.314eb63de3190b5c67ec0404713d114bf84982290a3926df437fe4e6bbc91062.a69c88568d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-05T16:56:20.496Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.46147c9df8be4c6e6757a1ac03c21c10010437ed01e6b97cb02a63e288b95d94.7a805b7fba^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>89a05e84d69405f7</t>
+  </si>
+  <si>
+    <t>2023-03-05T17:01:07.926Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.90e07a68edba97bdada97a413d58c7472d053d5c35c9b18b309a04dcdbf78cdd.1b246fd391^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>eaa0473038ce8ba0</t>
+  </si>
+  <si>
+    <t>2023-03-05T17:07:00.384Z</t>
+  </si>
+  <si>
+    <t>3b318c24c630023f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.ab91a5e7d8ddeb94390843ddb59539618c556060e3fb14bd38a68389244498c6.eb7f903839^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-05T17:16:25.373Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.de33c6b31ef81fea3bd871de1a0ea6fbfdb5bcdc7431723e1bf740d64399681d.f8b9cd915c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>bf79505e355cf773</t>
+  </si>
+  <si>
+    <t>2023-03-06T07:47:33.977Z</t>
+  </si>
+  <si>
+    <t>996e559a7f14bb0f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.7ef242a95da7abdcccfd50cca1c10c6c82f9e6e619dfa576a08899c4ec871028.48090ed2db^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-06T08:00:03.949Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.e028c855b330653cee54911be69fe1e432ab7a025b16d0cf93832c612ef6f346.45d56d695c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>599c8db14a96e9d6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.c6f6d53d1cf18f64eafa5de3c958d9170ef1ae2dd611c6a67f643a5f8cb0310a.16b87a2d3d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-06T08:08:29.254Z</t>
+  </si>
+  <si>
+    <t>78a47e19da1a59f2</t>
+  </si>
+  <si>
+    <t>2023-03-06T08:18:01.907Z</t>
+  </si>
+  <si>
+    <t>f4b8acd4511388cb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.a69b4b834dbb344d212afe4ff0cc277a681ac752b68104d49b0914f1ad9a6eb0.1c96c10c32^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2152,9 +2174,7 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -2522,7 +2542,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -2629,7 +2649,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="11" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2653,6 +2673,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4021,11 +4044,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O992"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E86" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="G92" sqref="G92:I92"/>
+      <selection pane="bottomRight" activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4080,7 +4103,7 @@
       </c>
       <c r="B3" s="49"/>
       <c r="C3" s="54" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="D3" s="46"/>
       <c r="F3" s="7"/>
@@ -4098,7 +4121,7 @@
       <c r="A4" s="50"/>
       <c r="B4" s="51"/>
       <c r="C4" s="54" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="D4" s="46"/>
       <c r="E4" s="2"/>
@@ -4117,7 +4140,7 @@
       <c r="A5" s="52"/>
       <c r="B5" s="53"/>
       <c r="C5" s="54" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="D5" s="46"/>
       <c r="F5" s="7"/>
@@ -4480,16 +4503,16 @@
         <v>48</v>
       </c>
       <c r="F19" s="17">
-        <v>44970</v>
+        <v>44991</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>321</v>
-      </c>
-      <c r="H19" s="18" t="s">
-        <v>322</v>
+        <v>409</v>
+      </c>
+      <c r="H19" s="55" t="s">
+        <v>410</v>
       </c>
       <c r="I19" s="18" t="s">
-        <v>323</v>
+        <v>411</v>
       </c>
       <c r="J19" s="19"/>
       <c r="K19" s="19" t="s">
@@ -4519,16 +4542,16 @@
         <v>50</v>
       </c>
       <c r="F20" s="17">
-        <v>44970</v>
+        <v>44991</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>324</v>
+        <v>412</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>325</v>
+        <v>414</v>
       </c>
       <c r="I20" s="18" t="s">
-        <v>326</v>
+        <v>413</v>
       </c>
       <c r="J20" s="19"/>
       <c r="K20" s="19" t="s">
@@ -4558,16 +4581,16 @@
         <v>52</v>
       </c>
       <c r="F21" s="17">
-        <v>44970</v>
+        <v>44991</v>
       </c>
       <c r="G21" s="38" t="s">
-        <v>374</v>
+        <v>416</v>
       </c>
       <c r="H21" s="38" t="s">
-        <v>375</v>
+        <v>417</v>
       </c>
       <c r="I21" s="38" t="s">
-        <v>373</v>
+        <v>415</v>
       </c>
       <c r="J21" s="19"/>
       <c r="K21" s="19" t="s">
@@ -4579,7 +4602,7 @@
       <c r="M21" s="19"/>
       <c r="N21" s="20"/>
       <c r="O21" s="40" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="135.75" thickBot="1">
@@ -4599,16 +4622,16 @@
         <v>54</v>
       </c>
       <c r="F22" s="17">
-        <v>44970</v>
+        <v>44991</v>
       </c>
       <c r="G22" s="38" t="s">
-        <v>378</v>
+        <v>418</v>
       </c>
       <c r="H22" s="38" t="s">
-        <v>377</v>
+        <v>419</v>
       </c>
       <c r="I22" s="38" t="s">
-        <v>376</v>
+        <v>420</v>
       </c>
       <c r="J22" s="19"/>
       <c r="K22" s="19" t="s">
@@ -4620,7 +4643,7 @@
       <c r="M22" s="19"/>
       <c r="N22" s="20"/>
       <c r="O22" s="40" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="135" hidden="1">
@@ -5015,7 +5038,7 @@
       <c r="C37" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="41" t="s">
         <v>87</v>
       </c>
       <c r="E37" s="16" t="s">
@@ -5025,16 +5048,16 @@
         <v>44970</v>
       </c>
       <c r="G37" s="38" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="H37" s="38" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="I37" s="38" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="J37" s="37" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="K37" s="19" t="s">
         <v>84</v>
@@ -5213,16 +5236,16 @@
         <v>44970</v>
       </c>
       <c r="G43" s="38" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="H43" s="38" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="I43" s="38" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="J43" s="37" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="K43" s="19" t="s">
         <v>84</v>
@@ -5397,14 +5420,12 @@
       <c r="E49" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="F49" s="17">
-        <v>44970</v>
-      </c>
+      <c r="F49" s="17"/>
       <c r="G49" s="18"/>
       <c r="H49" s="18"/>
       <c r="I49" s="18"/>
       <c r="J49" s="37" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="K49" s="19" t="s">
         <v>84</v>
@@ -6189,19 +6210,19 @@
         <v>160</v>
       </c>
       <c r="F76" s="17">
-        <v>44970</v>
+        <v>44990</v>
       </c>
       <c r="G76" s="38" t="s">
-        <v>339</v>
+        <v>361</v>
       </c>
       <c r="H76" s="38" t="s">
-        <v>340</v>
+        <v>362</v>
       </c>
       <c r="I76" s="38" t="s">
+        <v>327</v>
+      </c>
+      <c r="J76" s="37" t="s">
         <v>333</v>
-      </c>
-      <c r="J76" s="37" t="s">
-        <v>341</v>
       </c>
       <c r="K76" s="19" t="s">
         <v>84</v>
@@ -6214,7 +6235,7 @@
         <v>84</v>
       </c>
       <c r="O76" s="39" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
     </row>
     <row r="77" spans="1:15" ht="120.75" thickBot="1">
@@ -6234,19 +6255,19 @@
         <v>162</v>
       </c>
       <c r="F77" s="17">
-        <v>44970</v>
+        <v>44990</v>
       </c>
       <c r="G77" s="38" t="s">
-        <v>343</v>
+        <v>364</v>
       </c>
       <c r="H77" s="38" t="s">
-        <v>344</v>
+        <v>366</v>
       </c>
       <c r="I77" s="38" t="s">
-        <v>345</v>
+        <v>365</v>
       </c>
       <c r="J77" s="37" t="s">
-        <v>346</v>
+        <v>363</v>
       </c>
       <c r="K77" s="19" t="s">
         <v>84</v>
@@ -6259,7 +6280,7 @@
         <v>84</v>
       </c>
       <c r="O77" s="39" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
     </row>
     <row r="78" spans="1:15" ht="225.75" thickBot="1">
@@ -6279,19 +6300,19 @@
         <v>164</v>
       </c>
       <c r="F78" s="17">
-        <v>44970</v>
+        <v>44990</v>
       </c>
       <c r="G78" s="38" t="s">
-        <v>351</v>
+        <v>367</v>
       </c>
       <c r="H78" s="38" t="s">
-        <v>350</v>
+        <v>369</v>
       </c>
       <c r="I78" s="38" t="s">
-        <v>349</v>
+        <v>368</v>
       </c>
       <c r="J78" s="37" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="K78" s="19" t="s">
         <v>84</v>
@@ -6304,7 +6325,7 @@
         <v>84</v>
       </c>
       <c r="O78" s="39" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
     </row>
     <row r="79" spans="1:15" ht="135.75" thickBot="1">
@@ -6317,26 +6338,26 @@
       <c r="C79" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D79" s="15" t="s">
+      <c r="D79" s="41" t="s">
         <v>165</v>
       </c>
       <c r="E79" s="16" t="s">
         <v>166</v>
       </c>
       <c r="F79" s="17">
-        <v>44970</v>
+        <v>44990</v>
       </c>
       <c r="G79" s="38" t="s">
-        <v>353</v>
+        <v>370</v>
       </c>
       <c r="H79" s="38" t="s">
-        <v>354</v>
+        <v>371</v>
       </c>
       <c r="I79" s="38" t="s">
-        <v>355</v>
+        <v>372</v>
       </c>
       <c r="J79" s="38" t="s">
-        <v>356</v>
+        <v>338</v>
       </c>
       <c r="K79" s="19" t="s">
         <v>84</v>
@@ -6349,7 +6370,7 @@
         <v>84</v>
       </c>
       <c r="O79" s="39" t="s">
-        <v>357</v>
+        <v>339</v>
       </c>
     </row>
     <row r="80" spans="1:15" ht="120.75" thickBot="1">
@@ -6369,19 +6390,19 @@
         <v>168</v>
       </c>
       <c r="F80" s="17">
-        <v>44970</v>
+        <v>44990</v>
       </c>
       <c r="G80" s="38" t="s">
-        <v>369</v>
-      </c>
-      <c r="H80" s="38" t="s">
-        <v>367</v>
+        <v>373</v>
+      </c>
+      <c r="H80" s="42" t="s">
+        <v>374</v>
       </c>
       <c r="I80" s="38" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
       <c r="J80" s="37" t="s">
-        <v>358</v>
+        <v>340</v>
       </c>
       <c r="K80" s="19" t="s">
         <v>84</v>
@@ -6394,7 +6415,7 @@
         <v>84</v>
       </c>
       <c r="O80" s="39" t="s">
-        <v>359</v>
+        <v>341</v>
       </c>
     </row>
     <row r="81" spans="1:15" ht="120.75" thickBot="1">
@@ -6414,19 +6435,19 @@
         <v>170</v>
       </c>
       <c r="F81" s="17">
-        <v>44970</v>
+        <v>44990</v>
       </c>
       <c r="G81" s="38" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
       <c r="H81" s="38" t="s">
-        <v>370</v>
+        <v>377</v>
       </c>
       <c r="I81" s="38" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="J81" s="37" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="K81" s="19" t="s">
         <v>84</v>
@@ -6439,7 +6460,7 @@
         <v>84</v>
       </c>
       <c r="O81" s="39" t="s">
-        <v>361</v>
+        <v>343</v>
       </c>
     </row>
     <row r="82" spans="1:15" ht="150.75" thickBot="1">
@@ -6459,19 +6480,19 @@
         <v>172</v>
       </c>
       <c r="F82" s="17">
-        <v>44970</v>
-      </c>
-      <c r="G82" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="H82" s="18" t="s">
-        <v>362</v>
-      </c>
-      <c r="I82" s="18" t="s">
-        <v>366</v>
+        <v>44990</v>
+      </c>
+      <c r="G82" s="38" t="s">
+        <v>379</v>
+      </c>
+      <c r="H82" s="38" t="s">
+        <v>381</v>
+      </c>
+      <c r="I82" s="38" t="s">
+        <v>380</v>
       </c>
       <c r="J82" s="19" t="s">
-        <v>364</v>
+        <v>344</v>
       </c>
       <c r="K82" s="19" t="s">
         <v>84</v>
@@ -6484,10 +6505,10 @@
         <v>84</v>
       </c>
       <c r="O82" s="39" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="83" spans="1:15" ht="210">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" ht="210.75" thickBot="1">
       <c r="A83" s="14">
         <v>82</v>
       </c>
@@ -6504,19 +6525,19 @@
         <v>174</v>
       </c>
       <c r="F83" s="17">
-        <v>44970</v>
-      </c>
-      <c r="G83" s="18" t="s">
-        <v>379</v>
-      </c>
-      <c r="H83" s="18" t="s">
-        <v>380</v>
-      </c>
-      <c r="I83" s="18" t="s">
-        <v>381</v>
+        <v>44990</v>
+      </c>
+      <c r="G83" s="38" t="s">
+        <v>383</v>
+      </c>
+      <c r="H83" s="38" t="s">
+        <v>384</v>
+      </c>
+      <c r="I83" s="38" t="s">
+        <v>382</v>
       </c>
       <c r="J83" s="19" t="s">
-        <v>382</v>
+        <v>346</v>
       </c>
       <c r="K83" s="19" t="s">
         <v>84</v>
@@ -6529,7 +6550,7 @@
         <v>84</v>
       </c>
       <c r="O83" s="39" t="s">
-        <v>383</v>
+        <v>347</v>
       </c>
     </row>
     <row r="84" spans="1:15" ht="225">
@@ -6549,19 +6570,19 @@
         <v>176</v>
       </c>
       <c r="F84" s="17">
-        <v>44970</v>
-      </c>
-      <c r="G84" s="18" t="s">
-        <v>384</v>
-      </c>
-      <c r="H84" s="18" t="s">
+        <v>44990</v>
+      </c>
+      <c r="G84" s="38" t="s">
         <v>385</v>
       </c>
-      <c r="I84" s="18" t="s">
+      <c r="H84" s="38" t="s">
         <v>386</v>
       </c>
+      <c r="I84" s="38" t="s">
+        <v>387</v>
+      </c>
       <c r="J84" s="19" t="s">
-        <v>387</v>
+        <v>348</v>
       </c>
       <c r="K84" s="19" t="s">
         <v>84</v>
@@ -6574,7 +6595,7 @@
         <v>84</v>
       </c>
       <c r="O84" s="21" t="s">
-        <v>388</v>
+        <v>349</v>
       </c>
     </row>
     <row r="85" spans="1:15" ht="165">
@@ -6594,19 +6615,19 @@
         <v>178</v>
       </c>
       <c r="F85" s="17">
-        <v>44970</v>
-      </c>
-      <c r="G85" s="18" t="s">
+        <v>44990</v>
+      </c>
+      <c r="G85" s="38" t="s">
+        <v>388</v>
+      </c>
+      <c r="H85" s="38" t="s">
+        <v>390</v>
+      </c>
+      <c r="I85" s="38" t="s">
         <v>389</v>
       </c>
-      <c r="H85" s="18" t="s">
-        <v>390</v>
-      </c>
-      <c r="I85" s="18" t="s">
-        <v>391</v>
-      </c>
       <c r="J85" s="19" t="s">
-        <v>392</v>
+        <v>350</v>
       </c>
       <c r="K85" s="19" t="s">
         <v>84</v>
@@ -6619,7 +6640,7 @@
         <v>84</v>
       </c>
       <c r="O85" s="21" t="s">
-        <v>393</v>
+        <v>351</v>
       </c>
     </row>
     <row r="86" spans="1:15" ht="120">
@@ -6639,19 +6660,19 @@
         <v>180</v>
       </c>
       <c r="F86" s="17">
-        <v>44970</v>
-      </c>
-      <c r="G86" s="18" t="s">
-        <v>394</v>
-      </c>
-      <c r="H86" s="18" t="s">
-        <v>395</v>
-      </c>
-      <c r="I86" s="18" t="s">
-        <v>396</v>
+        <v>44990</v>
+      </c>
+      <c r="G86" s="38" t="s">
+        <v>391</v>
+      </c>
+      <c r="H86" s="38" t="s">
+        <v>392</v>
+      </c>
+      <c r="I86" s="38" t="s">
+        <v>393</v>
       </c>
       <c r="J86" s="19" t="s">
-        <v>397</v>
+        <v>352</v>
       </c>
       <c r="K86" s="19" t="s">
         <v>84</v>
@@ -6664,7 +6685,7 @@
         <v>84</v>
       </c>
       <c r="O86" s="21" t="s">
-        <v>398</v>
+        <v>353</v>
       </c>
     </row>
     <row r="87" spans="1:15" ht="120.75" thickBot="1">
@@ -6684,19 +6705,19 @@
         <v>182</v>
       </c>
       <c r="F87" s="17">
-        <v>44970</v>
-      </c>
-      <c r="G87" s="18" t="s">
-        <v>399</v>
-      </c>
-      <c r="H87" s="18" t="s">
-        <v>400</v>
-      </c>
-      <c r="I87" s="18" t="s">
-        <v>401</v>
+        <v>44990</v>
+      </c>
+      <c r="G87" s="38" t="s">
+        <v>394</v>
+      </c>
+      <c r="H87" s="38" t="s">
+        <v>395</v>
+      </c>
+      <c r="I87" s="38" t="s">
+        <v>396</v>
       </c>
       <c r="J87" s="37" t="s">
-        <v>402</v>
+        <v>354</v>
       </c>
       <c r="K87" s="19" t="s">
         <v>84</v>
@@ -6709,7 +6730,7 @@
         <v>84</v>
       </c>
       <c r="O87" s="21" t="s">
-        <v>403</v>
+        <v>355</v>
       </c>
     </row>
     <row r="88" spans="1:15" ht="135.75" thickBot="1">
@@ -6729,19 +6750,19 @@
         <v>184</v>
       </c>
       <c r="F88" s="17">
-        <v>44970</v>
+        <v>44990</v>
       </c>
       <c r="G88" s="38" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="H88" s="38" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="I88" s="38" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="J88" s="37" t="s">
-        <v>410</v>
+        <v>356</v>
       </c>
       <c r="K88" s="19" t="s">
         <v>84</v>
@@ -6772,19 +6793,19 @@
         <v>186</v>
       </c>
       <c r="F89" s="17">
-        <v>44970</v>
+        <v>44990</v>
       </c>
       <c r="G89" s="38" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="H89" s="38" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="I89" s="38" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="J89" s="37" t="s">
-        <v>411</v>
+        <v>357</v>
       </c>
       <c r="K89" s="19" t="s">
         <v>84</v>
@@ -6798,7 +6819,7 @@
       </c>
       <c r="O89" s="21"/>
     </row>
-    <row r="90" spans="1:15" ht="105">
+    <row r="90" spans="1:15" ht="105.75" thickBot="1">
       <c r="A90" s="14">
         <v>89</v>
       </c>
@@ -6824,7 +6845,7 @@
       </c>
       <c r="L90" s="19"/>
       <c r="M90" s="37" t="s">
-        <v>412</v>
+        <v>358</v>
       </c>
       <c r="N90" s="20" t="s">
         <v>84</v>
@@ -6857,7 +6878,7 @@
       </c>
       <c r="L91" s="19"/>
       <c r="M91" s="37" t="s">
-        <v>419</v>
+        <v>360</v>
       </c>
       <c r="N91" s="20" t="s">
         <v>84</v>
@@ -6890,7 +6911,7 @@
       </c>
       <c r="L92" s="19"/>
       <c r="M92" s="37" t="s">
-        <v>419</v>
+        <v>360</v>
       </c>
       <c r="N92" s="20" t="s">
         <v>84</v>
@@ -6914,19 +6935,19 @@
         <v>194</v>
       </c>
       <c r="F93" s="17">
-        <v>44970</v>
-      </c>
-      <c r="G93" s="18" t="s">
-        <v>414</v>
-      </c>
-      <c r="H93" s="18" t="s">
-        <v>413</v>
-      </c>
-      <c r="I93" s="18" t="s">
-        <v>415</v>
+        <v>44990</v>
+      </c>
+      <c r="G93" s="38" t="s">
+        <v>403</v>
+      </c>
+      <c r="H93" s="38" t="s">
+        <v>404</v>
+      </c>
+      <c r="I93" s="38" t="s">
+        <v>405</v>
       </c>
       <c r="J93" s="37" t="s">
-        <v>416</v>
+        <v>359</v>
       </c>
       <c r="K93" s="19" t="s">
         <v>84</v>
@@ -6957,19 +6978,19 @@
         <v>196</v>
       </c>
       <c r="F94" s="17">
-        <v>44970</v>
-      </c>
-      <c r="G94" s="42" t="s">
-        <v>418</v>
+        <v>44990</v>
+      </c>
+      <c r="G94" s="38" t="s">
+        <v>406</v>
       </c>
       <c r="H94" s="38" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="I94" s="38" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="J94" s="37" t="s">
-        <v>364</v>
+        <v>344</v>
       </c>
       <c r="K94" s="37" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
Aggiunot Attributo ID alle section
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111ELCO0000000/EL_CO_/Fenix/v3_19_05/report-checklist.xlsx
+++ b/GATEWAY/A1#111ELCO0000000/EL_CO_/Fenix/v3_19_05/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio.capra\Desktop\ACCREDITAMENTO\A1#111ELCO0000000\EL_CO_\Fenix\v3_19_05\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio.capra\Desktop\ACCREDITAMENTO\ACCREDITAMENTO_FSE\it-fse-accreditamento\GATEWAY\A1#111ELCO0000000\EL_CO_\Fenix\v3_19_05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9883D6-7FD7-424F-8503-91E40FED603A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A26469B-36CB-4796-B7F6-5CF47ED75FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5385" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2069,40 +2069,40 @@
     <t>bf79505e355cf773</t>
   </si>
   <si>
-    <t>2023-03-06T07:47:33.977Z</t>
-  </si>
-  <si>
-    <t>996e559a7f14bb0f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.7ef242a95da7abdcccfd50cca1c10c6c82f9e6e619dfa576a08899c4ec871028.48090ed2db^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-06T08:00:03.949Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.e028c855b330653cee54911be69fe1e432ab7a025b16d0cf93832c612ef6f346.45d56d695c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>599c8db14a96e9d6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.c6f6d53d1cf18f64eafa5de3c958d9170ef1ae2dd611c6a67f643a5f8cb0310a.16b87a2d3d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-06T08:08:29.254Z</t>
-  </si>
-  <si>
-    <t>78a47e19da1a59f2</t>
-  </si>
-  <si>
-    <t>2023-03-06T08:18:01.907Z</t>
-  </si>
-  <si>
-    <t>f4b8acd4511388cb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.a69b4b834dbb344d212afe4ff0cc277a681ac752b68104d49b0914f1ad9a6eb0.1c96c10c32^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-03-07T11:38:37.067Z</t>
+  </si>
+  <si>
+    <t>c38b19840fb88a1c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.733147c1eb24de4496c825722c49d84dfadd61e2b83fef64dbd7aa9798f6c2ae.5235aaf013^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-07T11:42:31.692Z</t>
+  </si>
+  <si>
+    <t>ac6d1809b5e03fdc</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.406160838b1fdc77624b49987030e0021620558c6851c2db8d7e658b5505592e.fa0e858790^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-07T11:55:12.829Z</t>
+  </si>
+  <si>
+    <t>52527e35e08478f6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.b11499c7fdb44d533fbabac7643f750c0eb861443d67e2e0365eb48bc12a4411.45210739a3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-07T12:00:33.455Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.7737a0606afa9b856678d3394e920dccb232e78641e333c1478e12bff6dea208.a0cc3bcbda^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>24d6a14b181a393a</t>
   </si>
 </sst>
 </file>
@@ -2652,6 +2652,9 @@
     <xf numFmtId="11" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2673,9 +2676,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4045,10 +4045,10 @@
   <dimension ref="A1:O992"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="N9" sqref="N9"/>
+      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4080,12 +4080,12 @@
       <c r="O1" s="6"/>
     </row>
     <row r="2" spans="1:15" ht="24" customHeight="1">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="46"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="47"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -4098,14 +4098,14 @@
       <c r="O2" s="6"/>
     </row>
     <row r="3" spans="1:15" ht="24" customHeight="1">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="54" t="s">
+      <c r="B3" s="50"/>
+      <c r="C3" s="55" t="s">
         <v>322</v>
       </c>
-      <c r="D3" s="46"/>
+      <c r="D3" s="47"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -4118,12 +4118,12 @@
       <c r="O3" s="6"/>
     </row>
     <row r="4" spans="1:15" ht="24" customHeight="1">
-      <c r="A4" s="50"/>
-      <c r="B4" s="51"/>
-      <c r="C4" s="54" t="s">
+      <c r="A4" s="51"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="55" t="s">
         <v>323</v>
       </c>
-      <c r="D4" s="46"/>
+      <c r="D4" s="47"/>
       <c r="E4" s="2"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -4137,12 +4137,12 @@
       <c r="O4" s="6"/>
     </row>
     <row r="5" spans="1:15" ht="24" customHeight="1">
-      <c r="A5" s="52"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="54" t="s">
+      <c r="A5" s="53"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="55" t="s">
         <v>324</v>
       </c>
-      <c r="D5" s="46"/>
+      <c r="D5" s="47"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -4155,8 +4155,8 @@
       <c r="O5" s="6"/>
     </row>
     <row r="6" spans="1:15" ht="24" customHeight="1">
-      <c r="A6" s="43"/>
-      <c r="B6" s="44"/>
+      <c r="A6" s="44"/>
+      <c r="B6" s="45"/>
       <c r="C6" s="10"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -4503,12 +4503,12 @@
         <v>48</v>
       </c>
       <c r="F19" s="17">
-        <v>44991</v>
+        <v>44992</v>
       </c>
       <c r="G19" s="18" t="s">
         <v>409</v>
       </c>
-      <c r="H19" s="55" t="s">
+      <c r="H19" s="43" t="s">
         <v>410</v>
       </c>
       <c r="I19" s="18" t="s">
@@ -4542,16 +4542,16 @@
         <v>50</v>
       </c>
       <c r="F20" s="17">
-        <v>44991</v>
+        <v>44992</v>
       </c>
       <c r="G20" s="18" t="s">
         <v>412</v>
       </c>
       <c r="H20" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="I20" s="18" t="s">
         <v>414</v>
-      </c>
-      <c r="I20" s="18" t="s">
-        <v>413</v>
       </c>
       <c r="J20" s="19"/>
       <c r="K20" s="19" t="s">
@@ -4581,16 +4581,16 @@
         <v>52</v>
       </c>
       <c r="F21" s="17">
-        <v>44991</v>
+        <v>44992</v>
       </c>
       <c r="G21" s="38" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="H21" s="38" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="I21" s="38" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="J21" s="19"/>
       <c r="K21" s="19" t="s">
@@ -4622,16 +4622,16 @@
         <v>54</v>
       </c>
       <c r="F22" s="17">
-        <v>44991</v>
+        <v>44992</v>
       </c>
       <c r="G22" s="38" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="H22" s="38" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="I22" s="38" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="J22" s="19"/>
       <c r="K22" s="19" t="s">

</xml_diff>

<commit_message>
Levato apice e messa l'anamnesi patologica familiare indicata nella mail di risposta
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111ELCO0000000/EL_CO_/Fenix/v3_19_05/report-checklist.xlsx
+++ b/GATEWAY/A1#111ELCO0000000/EL_CO_/Fenix/v3_19_05/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio.capra\Desktop\ACCREDITAMENTO\ACCREDITAMENTO_FSE\it-fse-accreditamento\GATEWAY\A1#111ELCO0000000\EL_CO_\Fenix\v3_19_05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5066AEE5-AFAB-4FD2-8570-E8C885364495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF26389-5756-4487-BAD5-3658FC6D02F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5385" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2087,22 +2087,22 @@
     <t>2.16.840.1.113883.2.9.2.10.4.4.12345.406160838b1fdc77624b49987030e0021620558c6851c2db8d7e658b5505592e.fa0e858790^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2023-03-08T17:47:05.853Z</t>
-  </si>
-  <si>
-    <t>b3c1ce88225f4bec</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.44059d66c052aa575c8fc6582905c6441d2f3a896778a867597580090e0bc63f.21c7e499ab^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.9b33887b76181d3dd29de152dd0166491b2376fde09471c5f081ccfd616b0f72.220ea1be72^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-08T17:53:22.492Z</t>
-  </si>
-  <si>
-    <t>42660883fe2bc300</t>
+    <t>2023-03-10T08:27:46.330Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.71110c4beca180b7d7d470abc58cc1595945c9cdc5e7f07bf50649da3daa6fb0.af7423fd29^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>ac6f3014eda680e6</t>
+  </si>
+  <si>
+    <t>2023-03-10T08:36:49.052Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.4.4.12345.d2bd52845b8eb1ce54fc3c495d9a64b10a4e74283eed78edb9c22014aada1ce3.fc11badc5c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>3279dad12507b213</t>
   </si>
 </sst>
 </file>
@@ -4045,7 +4045,7 @@
   <dimension ref="A1:O992"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
@@ -4581,16 +4581,16 @@
         <v>52</v>
       </c>
       <c r="F21" s="17">
-        <v>44993</v>
+        <v>44995</v>
       </c>
       <c r="G21" s="38" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H21" s="38" t="s">
         <v>420</v>
       </c>
       <c r="I21" s="38" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="J21" s="19"/>
       <c r="K21" s="19" t="s">
@@ -4622,16 +4622,16 @@
         <v>54</v>
       </c>
       <c r="F22" s="17">
-        <v>44993</v>
+        <v>44995</v>
       </c>
       <c r="G22" s="38" t="s">
         <v>415</v>
       </c>
       <c r="H22" s="38" t="s">
+        <v>417</v>
+      </c>
+      <c r="I22" s="38" t="s">
         <v>416</v>
-      </c>
-      <c r="I22" s="38" t="s">
-        <v>417</v>
       </c>
       <c r="J22" s="19"/>
       <c r="K22" s="19" t="s">

</xml_diff>